<commit_message>
clean up of hts forms and associated workflow
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_retest_test.xlsx
+++ b/config/default/forms/app/hts_retest_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -1308,6 +1308,24 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="1"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFB7B7B7"/>
       </font>
@@ -1348,20 +1366,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <strike val="1"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFC27BA0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1403,26 +1423,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1497,7 +1497,7 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1505,20 +1505,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.5612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="82.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1377551020408"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="33.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="16.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="69.9234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.9948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.9795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="85.9438775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.6479591836735"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="34.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="16.6479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5360,2005 +5360,2005 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$1058, "begin group") = COUNTIF($A$1:$A$1058, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1049, "begin group") = COUNTIF($A$1:$A$1058, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="5"/>
+    <cfRule type="notContainsText" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="8" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="8" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="5"/>
+    <cfRule type="notContainsText" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="11" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="11" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="5"/>
+    <cfRule type="notContainsText" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="14" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="14" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="15" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="containsText" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A29="begin group", NOT($B29 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A29="end group", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A29="begin repeat", NOT($B29 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A29="end repeat", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I31">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I30 = "", $A30 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C31">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A30 = "end group"), NOT($A30 = "end repeat"), NOT($A30 = "")), $C30 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B31">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A30 = "end group"), NOT($A30 = "end repeat"), NOT($A30 = "")), $B30 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:A31">
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B31">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1057,B30)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H31">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G30 = ""), $H30 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="containsText" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A30="begin group", NOT($B30 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A30="end group", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $G30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A30="begin repeat", NOT($B30 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E31">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A30="end repeat", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $G30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I33 = "", $A33 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A33 = "end group"), NOT($A33 = "end repeat"), NOT($A33 = "")), $C33 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A33 = "end group"), NOT($A33 = "end repeat"), NOT($A33 = "")), $B33 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B33)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G33 = ""), $H33 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A33="begin group", NOT($B33 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A33="end group", $B33 = "", $C33 = "", $D33 = "", $E33 = "", $F33 = "", $G33 = "", $H33 = "", $I33 = "", $J33 = "", $K33 = "", $L33 = "", $M33 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A33="begin repeat", NOT($B33 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A33="end repeat", $B33 = "", $C33 = "", $D33 = "", $E33 = "", $F33 = "", $G33 = "", $H33 = "", $I33 = "", $J33 = "", $K33 = "", $L33 = "", $M33 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsText" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A32="begin group", NOT($B32 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A32="end group", $B32 = "", $C32 = "", $D32 = "", $E32 = "", $F32 = "", $G32 = "", $H32 = "", $I32 = "", $J32 = "", $K32 = "", $L32 = "", $M32 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A32="begin repeat", NOT($B32 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A32="end repeat", $B32 = "", $C32 = "", $D32 = "", $E32 = "", $F32 = "", $G32 = "", $H32 = "", $I32 = "", $J32 = "", $K32 = "", $L32 = "", $M32 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I35 = "", $A35 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $B35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1055,B35)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G35 = ""), $H35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I36 = "", $A36 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1054,B36)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I38 = "", $A38 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $B38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1054,B38)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A38="begin group", NOT($B38 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A38="end group", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $L38 = "", $M38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A38="begin repeat", NOT($B38 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A38="end repeat", $B38 = "", $C38 = "", $D38 = "", $E38 = "", $F38 = "", $G38 = "", $H38 = "", $I38 = "", $J38 = "", $K38 = "", $L38 = "", $M38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I39 = "", $A39 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A39 = "end group"), NOT($A39 = "end repeat"), NOT($A39 = "")), $C39 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A39 = "end group"), NOT($A39 = "end repeat"), NOT($A39 = "")), $B39 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39">
-    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1053,B39)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G39 = ""), $H39 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="containsText" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A39="begin group", NOT($B39 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A39="end group", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A39="begin repeat", NOT($B39 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A39="end repeat", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="cellIs" priority="106" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="106" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="containsText" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A40="begin group", NOT($B40 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A40="end group", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="cellIs" priority="110" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="110" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="cellIs" priority="111" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="111" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A40="begin repeat", NOT($B40 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A40="end repeat", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="containsText" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="cellIs" priority="117" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="117" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="containsText" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="cellIs" priority="124" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="124" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I45">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I43 = "", $A43 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C45">
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B45">
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $B43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:A45">
-    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B45">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1044,B43)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H45">
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G43 = ""), $H43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:Y45">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="containsText" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="cellIs" priority="137" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="137" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="containsText" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A53="begin group", NOT($B53 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A53="end group", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" priority="144" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="144" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" priority="145" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="145" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A53="begin repeat", NOT($B53 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A53="end repeat", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="containsText" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="cellIs" priority="151" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="151" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:I52">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I50 = "", $A50 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C52">
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $C50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $B50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:A52">
-    <cfRule type="cellIs" priority="155" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="155" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1038,B50)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:H52">
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G50 = ""), $H50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:Y52">
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $L50 = "", $M50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="containsText" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A47="begin group", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A47="end group", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" priority="163" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="163" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A47="begin repeat", NOT($B47 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A47="end repeat", $B47 = "", $C47 = "", $D47 = "", $E47 = "", $F47 = "", $G47 = "", $H47 = "", $I47 = "", $J47 = "", $K47 = "", $L47 = "", $M47 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="containsText" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A54="begin group", NOT($B54 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A54="end group", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I54 = "", $A54 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $C54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $B54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1044,B54)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G54 = ""), $H54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A54="begin repeat", NOT($B54 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A54="end repeat", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I55 = "", $A55 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $C55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $B55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="cellIs" priority="181" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="181" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1053,B55)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G55 = ""), $H55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A55="begin group", NOT($B55 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A55="end group", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" priority="187" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="187" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A55="begin repeat", NOT($B55 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A55="end repeat", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I56 = "", $A56 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A56 = "end group"), NOT($A56 = "end repeat"), NOT($A56 = "")), $C56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56:B57">
-    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A56 = "end group"), NOT($A56 = "end repeat"), NOT($A56 = "")), $B56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A57">
-    <cfRule type="cellIs" priority="193" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="193" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56:B57">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1052,B56)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:H57">
-    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G56 = ""), $H56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="containsText" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A56="begin group", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A56="end group", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="cellIs" priority="199" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="199" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A56="begin repeat", NOT($B56 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A56="end repeat", $B56 = "", $C56 = "", $D56 = "", $E56 = "", $F56 = "", $G56 = "", $H56 = "", $I56 = "", $J56 = "", $K56 = "", $L56 = "", $M56 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="containsText" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="cellIs" priority="205" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="205" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I48 = "", $A48 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $C48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A48 = "end group"), NOT($A48 = "end repeat"), NOT($A48 = "")), $B48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48">
-    <cfRule type="cellIs" priority="209" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="209" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B48)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G48 = ""), $H48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:Y48">
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A48="end repeat", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $L48 = "", $M48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="containsText" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A41="begin group", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A41="end group", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="cellIs" priority="217" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="217" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I41 = "", $A41 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $C41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $B41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="cellIs" priority="221" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="221" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1055,B41)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G41 = ""), $H41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A41="begin repeat", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:Y41">
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A41="end repeat", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="containsText" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A78="begin group", NOT($B78 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A78="end group", $B78 = "", $C78 = "", $D78 = "", $E78 = "", $F78 = "", $G78 = "", $H78 = "", $I78 = "", $J78 = "", $K78 = "", $L78 = "", $M78 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="cellIs" priority="229" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="229" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A78="begin repeat", NOT($B78 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:E89">
-    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A78="end repeat", $B78 = "", $C78 = "", $D78 = "", $E78 = "", $F78 = "", $G78 = "", $H78 = "", $I78 = "", $J78 = "", $K78 = "", $L78 = "", $M78 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I89">
-    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I89 = "", $A89 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A89 = "end group"), NOT($A89 = "end repeat"), NOT($A89 = "")), $C89 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A89 = "end group"), NOT($A89 = "end repeat"), NOT($A89 = "")), $B89 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89">
-    <cfRule type="cellIs" priority="235" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="235" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B89)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G89 = ""), $H89 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="containsText" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A91="begin group", NOT($B91 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A91="end group", $B91 = "", $C91 = "", $D91 = "", $E91 = "", $F91 = "", $G91 = "", $H91 = "", $I91 = "", $J91 = "", $K91 = "", $L91 = "", $M91 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="cellIs" priority="241" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="241" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I91">
-    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I91 = "", $A91 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A91 = "end group"), NOT($A91 = "end repeat"), NOT($A91 = "")), $C91 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A91 = "end group"), NOT($A91 = "end repeat"), NOT($A91 = "")), $B91 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91">
-    <cfRule type="cellIs" priority="245" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="245" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B91)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91">
-    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G91 = ""), $H91 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A91="begin repeat", NOT($B91 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:Y91">
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A91="end repeat", $B91 = "", $C91 = "", $D91 = "", $E91 = "", $F91 = "", $G91 = "", $H91 = "", $I91 = "", $J91 = "", $K91 = "", $L91 = "", $M91 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="containsText" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A92="begin group", NOT($B92 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A92="end group", $B92 = "", $C92 = "", $D92 = "", $E92 = "", $F92 = "", $G92 = "", $H92 = "", $I92 = "", $J92 = "", $K92 = "", $L92 = "", $M92 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="cellIs" priority="253" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="253" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I92">
-    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I92 = "", $A92 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A92 = "end group"), NOT($A92 = "end repeat"), NOT($A92 = "")), $C92 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A92 = "end group"), NOT($A92 = "end repeat"), NOT($A92 = "")), $B92 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92">
-    <cfRule type="cellIs" priority="257" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="257" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1055,B92)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G92 = ""), $H92 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A92="begin repeat", NOT($B92 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:Y92">
-    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A92="end repeat", $B92 = "", $C92 = "", $D92 = "", $E92 = "", $F92 = "", $G92 = "", $H92 = "", $I92 = "", $J92 = "", $K92 = "", $L92 = "", $M92 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="containsText" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A94="begin group", NOT($B94 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A94="end group", $B94 = "", $C94 = "", $D94 = "", $E94 = "", $F94 = "", $G94 = "", $H94 = "", $I94 = "", $J94 = "", $K94 = "", $L94 = "", $M94 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="cellIs" priority="265" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="265" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I94">
-    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I94 = "", $A94 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A94 = "end group"), NOT($A94 = "end repeat"), NOT($A94 = "")), $C94 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A94 = "end group"), NOT($A94 = "end repeat"), NOT($A94 = "")), $B94 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94">
-    <cfRule type="cellIs" priority="269" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="269" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="expression" priority="270" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="270" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1054,B94)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H94">
-    <cfRule type="expression" priority="271" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="271" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G94 = ""), $H94 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="expression" priority="272" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="272" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A94="begin repeat", NOT($B94 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A94:Y94">
-    <cfRule type="expression" priority="273" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="273" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A94="end repeat", $B94 = "", $C94 = "", $D94 = "", $E94 = "", $F94 = "", $G94 = "", $H94 = "", $I94 = "", $J94 = "", $K94 = "", $L94 = "", $M94 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="containsText" priority="274" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="274" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="expression" priority="275" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="275" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A95="begin group", NOT($B95 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="expression" priority="276" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="276" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A95="end group", $B95 = "", $C95 = "", $D95 = "", $E95 = "", $F95 = "", $G95 = "", $H95 = "", $I95 = "", $J95 = "", $K95 = "", $L95 = "", $M95 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="cellIs" priority="277" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="277" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I95">
-    <cfRule type="expression" priority="278" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="278" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I95 = "", $A95 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" priority="279" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="279" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A95 = "end group"), NOT($A95 = "end repeat"), NOT($A95 = "")), $C95 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="expression" priority="280" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="280" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A95 = "end group"), NOT($A95 = "end repeat"), NOT($A95 = "")), $B95 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95">
-    <cfRule type="cellIs" priority="281" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="281" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="expression" priority="282" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="282" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1053,B95)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95">
-    <cfRule type="expression" priority="283" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="283" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G95 = ""), $H95 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="expression" priority="284" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="284" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A95="begin repeat", NOT($B95 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:Y95">
-    <cfRule type="expression" priority="285" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="285" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A95="end repeat", $B95 = "", $C95 = "", $D95 = "", $E95 = "", $F95 = "", $G95 = "", $H95 = "", $I95 = "", $J95 = "", $K95 = "", $L95 = "", $M95 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="containsText" priority="286" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="286" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="expression" priority="287" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="287" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A96="begin group", NOT($B96 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="expression" priority="288" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="288" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A96="end group", $B96 = "", $C96 = "", $D96 = "", $E96 = "", $F96 = "", $G96 = "", $H96 = "", $I96 = "", $J96 = "", $K96 = "", $L96 = "", $M96 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="cellIs" priority="289" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="289" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I96">
-    <cfRule type="expression" priority="290" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="290" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I96 = "", $A96 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" priority="291" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="291" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A96 = "end group"), NOT($A96 = "end repeat"), NOT($A96 = "")), $C96 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="expression" priority="292" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="292" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A96 = "end group"), NOT($A96 = "end repeat"), NOT($A96 = "")), $B96 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96">
-    <cfRule type="cellIs" priority="293" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="293" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="expression" priority="294" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="294" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1052,B96)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H96">
-    <cfRule type="expression" priority="295" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="295" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G96 = ""), $H96 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="expression" priority="296" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="296" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A96="begin repeat", NOT($B96 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:Y96">
-    <cfRule type="expression" priority="297" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="297" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A96="end repeat", $B96 = "", $C96 = "", $D96 = "", $E96 = "", $F96 = "", $G96 = "", $H96 = "", $I96 = "", $J96 = "", $K96 = "", $L96 = "", $M96 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="containsText" priority="298" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="298" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="expression" priority="299" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="299" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A98="begin group", NOT($B98 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="expression" priority="300" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="300" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A98="end group", $B98 = "", $C98 = "", $D98 = "", $E98 = "", $F98 = "", $G98 = "", $H98 = "", $I98 = "", $J98 = "", $K98 = "", $L98 = "", $M98 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="cellIs" priority="301" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="301" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98">
-    <cfRule type="expression" priority="302" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="302" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I98 = "", $A98 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" priority="303" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="303" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A98 = "end group"), NOT($A98 = "end repeat"), NOT($A98 = "")), $C98 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" priority="304" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="304" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A98 = "end group"), NOT($A98 = "end repeat"), NOT($A98 = "")), $B98 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98">
-    <cfRule type="cellIs" priority="305" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="305" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" priority="306" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="306" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1051,B98)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="expression" priority="307" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="307" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G98 = ""), $H98 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="expression" priority="308" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="308" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A98="begin repeat", NOT($B98 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:Y98">
-    <cfRule type="expression" priority="309" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="309" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A98="end repeat", $B98 = "", $C98 = "", $D98 = "", $E98 = "", $F98 = "", $G98 = "", $H98 = "", $I98 = "", $J98 = "", $K98 = "", $L98 = "", $M98 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="containsText" priority="310" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="310" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="expression" priority="311" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="311" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A99="begin group", NOT($B99 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="expression" priority="312" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="312" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A99="end group", $B99 = "", $C99 = "", $D99 = "", $E99 = "", $F99 = "", $G99 = "", $H99 = "", $I99 = "", $J99 = "", $K99 = "", $L99 = "", $M99 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="cellIs" priority="313" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="313" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I99">
-    <cfRule type="expression" priority="314" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="314" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I99 = "", $A99 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" priority="315" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="315" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A99 = "end group"), NOT($A99 = "end repeat"), NOT($A99 = "")), $C99 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" priority="316" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="316" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A99 = "end group"), NOT($A99 = "end repeat"), NOT($A99 = "")), $B99 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99">
-    <cfRule type="cellIs" priority="317" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="317" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" priority="318" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="318" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1050,B99)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99">
-    <cfRule type="expression" priority="319" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="319" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G99 = ""), $H99 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="expression" priority="320" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="320" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A99="begin repeat", NOT($B99 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:Y99">
-    <cfRule type="expression" priority="321" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="321" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A99="end repeat", $B99 = "", $C99 = "", $D99 = "", $E99 = "", $F99 = "", $G99 = "", $H99 = "", $I99 = "", $J99 = "", $K99 = "", $L99 = "", $M99 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="containsText" priority="322" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="322" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="expression" priority="323" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="323" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A100="begin group", NOT($B100 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="expression" priority="324" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="324" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A100="end group", $B100 = "", $C100 = "", $D100 = "", $E100 = "", $F100 = "", $G100 = "", $H100 = "", $I100 = "", $J100 = "", $K100 = "", $L100 = "", $M100 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="cellIs" priority="325" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="325" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I100">
-    <cfRule type="expression" priority="326" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="326" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I100 = "", $A100 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="expression" priority="327" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="327" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A100 = "end group"), NOT($A100 = "end repeat"), NOT($A100 = "")), $C100 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100">
-    <cfRule type="expression" priority="328" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="328" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A100 = "end group"), NOT($A100 = "end repeat"), NOT($A100 = "")), $B100 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100">
-    <cfRule type="cellIs" priority="329" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="329" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100">
-    <cfRule type="expression" priority="330" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="330" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1049,B100)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H100">
-    <cfRule type="expression" priority="331" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="331" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G100 = ""), $H100 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="expression" priority="332" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="332" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A100="begin repeat", NOT($B100 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:Y100">
-    <cfRule type="expression" priority="333" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="333" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A100="end repeat", $B100 = "", $C100 = "", $D100 = "", $E100 = "", $F100 = "", $G100 = "", $H100 = "", $I100 = "", $J100 = "", $K100 = "", $L100 = "", $M100 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="containsText" priority="334" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="334" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="expression" priority="335" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="335" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A105="begin group", NOT($B105 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="expression" priority="336" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="336" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A105="end group", $B105 = "", $C105 = "", $D105 = "", $E105 = "", $F105 = "", $G105 = "", $H105 = "", $I105 = "", $J105 = "", $K105 = "", $L105 = "", $M105 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="cellIs" priority="337" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="337" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I105">
-    <cfRule type="expression" priority="338" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="338" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I105 = "", $A105 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" priority="339" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="339" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A105 = "end group"), NOT($A105 = "end repeat"), NOT($A105 = "")), $C105 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" priority="340" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="340" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A105 = "end group"), NOT($A105 = "end repeat"), NOT($A105 = "")), $B105 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="cellIs" priority="341" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="341" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" priority="342" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="342" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B105)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="expression" priority="343" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="343" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G105 = ""), $H105 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="expression" priority="344" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="344" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A105="begin repeat", NOT($B105 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:Y105">
-    <cfRule type="expression" priority="345" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="345" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A105="end repeat", $B105 = "", $C105 = "", $D105 = "", $E105 = "", $F105 = "", $G105 = "", $H105 = "", $I105 = "", $J105 = "", $K105 = "", $L105 = "", $M105 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="containsText" priority="346" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="346" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="expression" priority="347" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="347" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A110="begin group", NOT($B110 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="expression" priority="348" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="348" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A110="end group", $B110 = "", $C110 = "", $D110 = "", $E110 = "", $F110 = "", $G110 = "", $H110 = "", $I110 = "", $J110 = "", $K110 = "", $L110 = "", $M110 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="cellIs" priority="349" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="349" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="cellIs" priority="350" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="350" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="expression" priority="351" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="351" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A110="begin repeat", NOT($B110 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110">
-    <cfRule type="expression" priority="352" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="352" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A110="end repeat", $B110 = "", $C110 = "", $D110 = "", $E110 = "", $F110 = "", $G110 = "", $H110 = "", $I110 = "", $J110 = "", $K110 = "", $L110 = "", $M110 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I102:I104">
-    <cfRule type="expression" priority="353" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="353" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I102 = "", $A102 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103:C104">
-    <cfRule type="expression" priority="354" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="354" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A103 = "end group"), NOT($A103 = "end repeat"), NOT($A103 = "")), $C103 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103:B104">
-    <cfRule type="expression" priority="355" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="355" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A103 = "end group"), NOT($A103 = "end repeat"), NOT($A103 = "")), $B103 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:A104">
-    <cfRule type="cellIs" priority="356" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="356" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103:B104">
-    <cfRule type="expression" priority="357" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="357" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1052,B103)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102:H104">
-    <cfRule type="expression" priority="358" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="358" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G102 = ""), $H102 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="containsText" priority="359" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="359" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="expression" priority="360" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="360" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A101="begin group", NOT($B101 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="expression" priority="361" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="361" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A101="end group", $B101 = "", $C101 = "", $D101 = "", $E101 = "", $F101 = "", $G101 = "", $H101 = "", $I101 = "", $J101 = "", $K101 = "", $L101 = "", $M101 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="cellIs" priority="362" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="362" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101">
-    <cfRule type="expression" priority="363" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="363" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I101 = "", $A101 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="expression" priority="364" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="364" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A101 = "end group"), NOT($A101 = "end repeat"), NOT($A101 = "")), $C101 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101">
-    <cfRule type="expression" priority="365" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="365" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A101 = "end group"), NOT($A101 = "end repeat"), NOT($A101 = "")), $B101 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101">
-    <cfRule type="cellIs" priority="366" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="366" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101">
-    <cfRule type="expression" priority="367" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="367" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1051,B101)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H101">
-    <cfRule type="expression" priority="368" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="368" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G101 = ""), $H101 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="expression" priority="369" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="369" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A101="begin repeat", NOT($B101 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:Y101">
-    <cfRule type="expression" priority="370" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="370" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A101="end repeat", $B101 = "", $C101 = "", $D101 = "", $E101 = "", $F101 = "", $G101 = "", $H101 = "", $I101 = "", $J101 = "", $K101 = "", $L101 = "", $M101 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" priority="371" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="371" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I37 = "", $A37 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" priority="372" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="372" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" priority="373" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="373" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" priority="374" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="374" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" priority="375" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="375" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1053,B37)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" priority="376" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="376" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" priority="377" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="377" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="378" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="378" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="379" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="379" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" priority="380" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="380" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="381" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="381" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="382" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="382" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="containsText" priority="383" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="383" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="384" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="384" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A93="begin group", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="385" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="385" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A93="end group", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" priority="386" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="386" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="387" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="387" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A93="begin repeat", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="388" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="388" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A93="end repeat", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="containsText" priority="389" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="389" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="390" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="390" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A93="begin group", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="391" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="391" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A93="end group", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" priority="392" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="392" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="393" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="393" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A93="begin repeat", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" priority="394" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="394" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A93="end repeat", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I93">
-    <cfRule type="expression" priority="395" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="395" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I93 = "", $A93 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" priority="396" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="396" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A93 = "end group"), NOT($A93 = "end repeat"), NOT($A93 = "")), $C93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" priority="397" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="397" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A93 = "end group"), NOT($A93 = "end repeat"), NOT($A93 = "")), $B93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93">
-    <cfRule type="cellIs" priority="398" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="398" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" priority="399" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="399" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1056,B93)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H93">
-    <cfRule type="expression" priority="400" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="400" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G93 = ""), $H93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="containsText" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A93="begin group", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A93="end group", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="405" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="405" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A93="begin repeat", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="406" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="406" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A93="end repeat", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="containsText" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A93="begin group", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="409" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="409" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A93="end group", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" priority="410" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="410" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A93="begin repeat", NOT($B93 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A93="end repeat", $B93 = "", $C93 = "", $D93 = "", $E93 = "", $F93 = "", $G93 = "", $H93 = "", $I93 = "", $J93 = "", $K93 = "", $L93 = "", $M93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I97">
-    <cfRule type="expression" priority="413" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="413" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($I93 = "", $A93 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(AND(NOT($A93 = "end group"), NOT($A93 = "end repeat"), NOT($A93 = "")), $C93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND(AND(NOT($A93 = "end group"), NOT($A93 = "end repeat"), NOT($A93 = "")), $B93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97">
-    <cfRule type="cellIs" priority="416" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="416" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>COUNTIF($B$2:$B$1055,B93)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97">
-    <cfRule type="expression" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>AND(NOT($G93 = ""), $H93 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7385,7 +7385,7 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
@@ -7393,10 +7393,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.6479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8498,7 +8498,7 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -8506,9 +8506,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.6479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="C2" s="13" t="n">
         <f aca="true">NOW()</f>
-        <v>43969.912729813</v>
+        <v>44033.9655296883</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>361</v>

</xml_diff>

<commit_message>
ipv workflow in contact listing
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_retest_test.xlsx
+++ b/config/default/forms/app/hts_retest_test.xlsx
@@ -1424,7 +1424,7 @@
     <t xml:space="preserve">_160579_msm_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Male who has sex with men</t>
+    <t xml:space="preserve">Men who have sex with men</t>
   </si>
   <si>
     <t xml:space="preserve">_159674_fisherfolk_99DCT</t>
@@ -1781,7 +1781,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1846,12 +1846,6 @@
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1979,7 +1973,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2028,23 +2022,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2084,27 +2074,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2112,11 +2102,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2124,7 +2114,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2137,16 +2127,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -2251,18 +2232,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="202.576530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.4285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.4285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="108.622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="248.382653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="82.8826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="79.015306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="99.265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="209.867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="112.581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="257.382653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="85.8571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="81.8061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="102.862244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6248,7 +6231,7 @@
       <c r="D116" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E116" s="12" t="s">
+      <c r="E116" s="8" t="s">
         <v>273</v>
       </c>
       <c r="F116" s="8"/>
@@ -6474,7 +6457,7 @@
       <c r="D122" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E122" s="12" t="s">
+      <c r="E122" s="8" t="s">
         <v>291</v>
       </c>
       <c r="F122" s="8"/>
@@ -6735,7 +6718,7 @@
       <c r="A130" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B130" s="13" t="s">
+      <c r="B130" s="12" t="s">
         <v>307</v>
       </c>
       <c r="C130" s="4" t="s">
@@ -6771,7 +6754,7 @@
       <c r="B131" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C131" s="13" t="s">
         <v>310</v>
       </c>
       <c r="D131" s="4"/>
@@ -6808,7 +6791,7 @@
       <c r="B132" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C132" s="14" t="s">
+      <c r="C132" s="13" t="s">
         <v>314</v>
       </c>
       <c r="D132" s="4"/>
@@ -6845,7 +6828,7 @@
       <c r="B133" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C133" s="14" t="s">
+      <c r="C133" s="13" t="s">
         <v>317</v>
       </c>
       <c r="D133" s="4"/>
@@ -6912,10 +6895,10 @@
       <c r="A135" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B135" s="14" t="s">
+      <c r="B135" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="C135" s="14" t="s">
+      <c r="C135" s="13" t="s">
         <v>322</v>
       </c>
       <c r="D135" s="4"/>
@@ -6949,10 +6932,10 @@
       <c r="A136" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="C136" s="14" t="s">
+      <c r="C136" s="13" t="s">
         <v>325</v>
       </c>
       <c r="D136" s="4"/>
@@ -6986,10 +6969,10 @@
       <c r="A137" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B137" s="14" t="s">
+      <c r="B137" s="13" t="s">
         <v>327</v>
       </c>
-      <c r="C137" s="14" t="s">
+      <c r="C137" s="13" t="s">
         <v>328</v>
       </c>
       <c r="D137" s="4"/>
@@ -7023,10 +7006,10 @@
       <c r="A138" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B138" s="14" t="s">
+      <c r="B138" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="C138" s="14" t="s">
+      <c r="C138" s="13" t="s">
         <v>331</v>
       </c>
       <c r="D138" s="4"/>
@@ -7060,10 +7043,10 @@
       <c r="A139" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B139" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="C139" s="14" t="s">
+      <c r="C139" s="13" t="s">
         <v>334</v>
       </c>
       <c r="D139" s="4"/>
@@ -7097,10 +7080,10 @@
       <c r="A140" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B140" s="14" t="s">
+      <c r="B140" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="C140" s="14" t="s">
+      <c r="C140" s="13" t="s">
         <v>337</v>
       </c>
       <c r="D140" s="4"/>
@@ -7134,10 +7117,10 @@
       <c r="A141" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B141" s="14" t="s">
+      <c r="B141" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="C141" s="14" t="s">
+      <c r="C141" s="13" t="s">
         <v>340</v>
       </c>
       <c r="D141" s="4"/>
@@ -7171,10 +7154,10 @@
       <c r="A142" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C142" s="14" t="s">
+      <c r="C142" s="13" t="s">
         <v>343</v>
       </c>
       <c r="D142" s="4"/>
@@ -7241,10 +7224,10 @@
       <c r="A144" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B144" s="14" t="s">
+      <c r="B144" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="C144" s="14" t="s">
+      <c r="C144" s="13" t="s">
         <v>348</v>
       </c>
       <c r="D144" s="4"/>
@@ -7278,10 +7261,10 @@
       <c r="A145" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B145" s="14" t="s">
+      <c r="B145" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="C145" s="14" t="s">
+      <c r="C145" s="13" t="s">
         <v>351</v>
       </c>
       <c r="D145" s="4"/>
@@ -7315,10 +7298,10 @@
       <c r="A146" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B146" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="C146" s="14" t="s">
+      <c r="C146" s="13" t="s">
         <v>354</v>
       </c>
       <c r="D146" s="4"/>
@@ -7352,10 +7335,10 @@
       <c r="A147" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B147" s="14" t="s">
+      <c r="B147" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C147" s="14" t="s">
+      <c r="C147" s="13" t="s">
         <v>357</v>
       </c>
       <c r="D147" s="4"/>
@@ -7389,10 +7372,10 @@
       <c r="A148" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="C148" s="14" t="s">
+      <c r="C148" s="13" t="s">
         <v>360</v>
       </c>
       <c r="D148" s="4"/>
@@ -7426,10 +7409,10 @@
       <c r="A149" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B149" s="14" t="s">
+      <c r="B149" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C149" s="14" t="s">
+      <c r="C149" s="13" t="s">
         <v>363</v>
       </c>
       <c r="D149" s="4"/>
@@ -7463,10 +7446,10 @@
       <c r="A150" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B150" s="14" t="s">
+      <c r="B150" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="C150" s="14" t="s">
+      <c r="C150" s="13" t="s">
         <v>366</v>
       </c>
       <c r="D150" s="4"/>
@@ -7500,10 +7483,10 @@
       <c r="A151" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B151" s="14" t="s">
+      <c r="B151" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="C151" s="14" t="s">
+      <c r="C151" s="13" t="s">
         <v>369</v>
       </c>
       <c r="D151" s="4"/>
@@ -7537,10 +7520,10 @@
       <c r="A152" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B152" s="14" t="s">
+      <c r="B152" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C152" s="14" t="s">
+      <c r="C152" s="13" t="s">
         <v>334</v>
       </c>
       <c r="D152" s="4"/>
@@ -7574,10 +7557,10 @@
       <c r="A153" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B153" s="14" t="s">
+      <c r="B153" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="C153" s="14" t="s">
+      <c r="C153" s="13" t="s">
         <v>374</v>
       </c>
       <c r="D153" s="4"/>
@@ -7611,10 +7594,10 @@
       <c r="A154" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B154" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="C154" s="14" t="s">
+      <c r="C154" s="13" t="s">
         <v>343</v>
       </c>
       <c r="D154" s="4"/>
@@ -8112,13 +8095,13 @@
       <c r="Y167" s="8"/>
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="15" t="s">
+      <c r="A168" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B168" s="14" t="s">
+      <c r="B168" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="C168" s="14" t="s">
+      <c r="C168" s="13" t="s">
         <v>410</v>
       </c>
       <c r="D168" s="4"/>
@@ -8128,99 +8111,99 @@
       <c r="F168" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G168" s="16"/>
-      <c r="H168" s="16"/>
-      <c r="I168" s="16"/>
-      <c r="J168" s="16"/>
-      <c r="K168" s="16"/>
-      <c r="L168" s="16"/>
-      <c r="M168" s="16"/>
-      <c r="N168" s="16"/>
-      <c r="O168" s="16"/>
-      <c r="P168" s="16"/>
-      <c r="Q168" s="16"/>
-      <c r="R168" s="16"/>
-      <c r="S168" s="16"/>
-      <c r="T168" s="16"/>
-      <c r="U168" s="16"/>
-      <c r="V168" s="16"/>
-      <c r="W168" s="16"/>
-      <c r="X168" s="16"/>
-      <c r="Y168" s="16"/>
+      <c r="G168" s="15"/>
+      <c r="H168" s="15"/>
+      <c r="I168" s="15"/>
+      <c r="J168" s="15"/>
+      <c r="K168" s="15"/>
+      <c r="L168" s="15"/>
+      <c r="M168" s="15"/>
+      <c r="N168" s="15"/>
+      <c r="O168" s="15"/>
+      <c r="P168" s="15"/>
+      <c r="Q168" s="15"/>
+      <c r="R168" s="15"/>
+      <c r="S168" s="15"/>
+      <c r="T168" s="15"/>
+      <c r="U168" s="15"/>
+      <c r="V168" s="15"/>
+      <c r="W168" s="15"/>
+      <c r="X168" s="15"/>
+      <c r="Y168" s="15"/>
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="15" t="s">
+      <c r="A169" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B169" s="14" t="s">
+      <c r="B169" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="C169" s="14" t="s">
+      <c r="C169" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="D169" s="16"/>
+      <c r="D169" s="15"/>
       <c r="E169" s="4" t="s">
         <v>414</v>
       </c>
       <c r="F169" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G169" s="16"/>
-      <c r="H169" s="16"/>
-      <c r="I169" s="16"/>
-      <c r="J169" s="16"/>
-      <c r="K169" s="16"/>
-      <c r="L169" s="16"/>
-      <c r="M169" s="16"/>
-      <c r="N169" s="16"/>
-      <c r="O169" s="16"/>
-      <c r="P169" s="16"/>
-      <c r="Q169" s="16"/>
-      <c r="R169" s="16"/>
-      <c r="S169" s="16"/>
-      <c r="T169" s="16"/>
-      <c r="U169" s="16"/>
-      <c r="V169" s="16"/>
-      <c r="W169" s="16"/>
-      <c r="X169" s="16"/>
-      <c r="Y169" s="16"/>
+      <c r="G169" s="15"/>
+      <c r="H169" s="15"/>
+      <c r="I169" s="15"/>
+      <c r="J169" s="15"/>
+      <c r="K169" s="15"/>
+      <c r="L169" s="15"/>
+      <c r="M169" s="15"/>
+      <c r="N169" s="15"/>
+      <c r="O169" s="15"/>
+      <c r="P169" s="15"/>
+      <c r="Q169" s="15"/>
+      <c r="R169" s="15"/>
+      <c r="S169" s="15"/>
+      <c r="T169" s="15"/>
+      <c r="U169" s="15"/>
+      <c r="V169" s="15"/>
+      <c r="W169" s="15"/>
+      <c r="X169" s="15"/>
+      <c r="Y169" s="15"/>
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="15" t="s">
+      <c r="A170" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B170" s="14" t="s">
+      <c r="B170" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="C170" s="14" t="s">
+      <c r="C170" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="D170" s="16"/>
+      <c r="D170" s="15"/>
       <c r="E170" s="4" t="s">
         <v>417</v>
       </c>
       <c r="F170" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G170" s="16"/>
-      <c r="H170" s="16"/>
-      <c r="I170" s="16"/>
-      <c r="J170" s="16"/>
-      <c r="K170" s="16"/>
-      <c r="L170" s="16"/>
-      <c r="M170" s="16"/>
-      <c r="N170" s="16"/>
-      <c r="O170" s="16"/>
-      <c r="P170" s="16"/>
-      <c r="Q170" s="16"/>
-      <c r="R170" s="16"/>
-      <c r="S170" s="16"/>
-      <c r="T170" s="16"/>
-      <c r="U170" s="16"/>
-      <c r="V170" s="16"/>
-      <c r="W170" s="16"/>
-      <c r="X170" s="16"/>
-      <c r="Y170" s="16"/>
+      <c r="G170" s="15"/>
+      <c r="H170" s="15"/>
+      <c r="I170" s="15"/>
+      <c r="J170" s="15"/>
+      <c r="K170" s="15"/>
+      <c r="L170" s="15"/>
+      <c r="M170" s="15"/>
+      <c r="N170" s="15"/>
+      <c r="O170" s="15"/>
+      <c r="P170" s="15"/>
+      <c r="Q170" s="15"/>
+      <c r="R170" s="15"/>
+      <c r="S170" s="15"/>
+      <c r="T170" s="15"/>
+      <c r="U170" s="15"/>
+      <c r="V170" s="15"/>
+      <c r="W170" s="15"/>
+      <c r="X170" s="15"/>
+      <c r="Y170" s="15"/>
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8" t="s">
@@ -8256,13 +8239,13 @@
       <c r="Y171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="15" t="s">
+      <c r="A172" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B172" s="14" t="s">
+      <c r="B172" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="C172" s="14" t="s">
+      <c r="C172" s="13" t="s">
         <v>421</v>
       </c>
       <c r="D172" s="4"/>
@@ -8272,108 +8255,108 @@
       <c r="F172" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G172" s="16"/>
-      <c r="H172" s="16"/>
-      <c r="I172" s="16"/>
-      <c r="J172" s="16"/>
-      <c r="K172" s="16"/>
-      <c r="L172" s="16"/>
-      <c r="M172" s="16"/>
-      <c r="N172" s="16"/>
-      <c r="O172" s="16"/>
-      <c r="P172" s="16"/>
-      <c r="Q172" s="16"/>
-      <c r="R172" s="16"/>
-      <c r="S172" s="16"/>
-      <c r="T172" s="16"/>
-      <c r="U172" s="16"/>
-      <c r="V172" s="16"/>
-      <c r="W172" s="16"/>
-      <c r="X172" s="16"/>
-      <c r="Y172" s="16"/>
+      <c r="G172" s="15"/>
+      <c r="H172" s="15"/>
+      <c r="I172" s="15"/>
+      <c r="J172" s="15"/>
+      <c r="K172" s="15"/>
+      <c r="L172" s="15"/>
+      <c r="M172" s="15"/>
+      <c r="N172" s="15"/>
+      <c r="O172" s="15"/>
+      <c r="P172" s="15"/>
+      <c r="Q172" s="15"/>
+      <c r="R172" s="15"/>
+      <c r="S172" s="15"/>
+      <c r="T172" s="15"/>
+      <c r="U172" s="15"/>
+      <c r="V172" s="15"/>
+      <c r="W172" s="15"/>
+      <c r="X172" s="15"/>
+      <c r="Y172" s="15"/>
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="15" t="s">
+      <c r="A173" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B173" s="14" t="s">
+      <c r="B173" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="C173" s="14" t="s">
+      <c r="C173" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="D173" s="16"/>
+      <c r="D173" s="15"/>
       <c r="E173" s="4" t="s">
         <v>425</v>
       </c>
       <c r="F173" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G173" s="16"/>
-      <c r="H173" s="16"/>
-      <c r="I173" s="16"/>
-      <c r="J173" s="16"/>
-      <c r="K173" s="16"/>
-      <c r="L173" s="16"/>
-      <c r="M173" s="16"/>
-      <c r="N173" s="16"/>
-      <c r="O173" s="16"/>
-      <c r="P173" s="16"/>
-      <c r="Q173" s="16"/>
-      <c r="R173" s="16"/>
-      <c r="S173" s="16"/>
-      <c r="T173" s="16"/>
-      <c r="U173" s="16"/>
-      <c r="V173" s="16"/>
-      <c r="W173" s="16"/>
-      <c r="X173" s="16"/>
-      <c r="Y173" s="16"/>
+      <c r="G173" s="15"/>
+      <c r="H173" s="15"/>
+      <c r="I173" s="15"/>
+      <c r="J173" s="15"/>
+      <c r="K173" s="15"/>
+      <c r="L173" s="15"/>
+      <c r="M173" s="15"/>
+      <c r="N173" s="15"/>
+      <c r="O173" s="15"/>
+      <c r="P173" s="15"/>
+      <c r="Q173" s="15"/>
+      <c r="R173" s="15"/>
+      <c r="S173" s="15"/>
+      <c r="T173" s="15"/>
+      <c r="U173" s="15"/>
+      <c r="V173" s="15"/>
+      <c r="W173" s="15"/>
+      <c r="X173" s="15"/>
+      <c r="Y173" s="15"/>
     </row>
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="15" t="s">
+      <c r="A174" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B174" s="14" t="s">
+      <c r="B174" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="C174" s="14" t="s">
+      <c r="C174" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="D174" s="16"/>
+      <c r="D174" s="15"/>
       <c r="E174" s="4" t="s">
         <v>428</v>
       </c>
       <c r="F174" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G174" s="16"/>
-      <c r="H174" s="16"/>
-      <c r="I174" s="16"/>
-      <c r="J174" s="16"/>
-      <c r="K174" s="16"/>
-      <c r="L174" s="16"/>
-      <c r="M174" s="16"/>
-      <c r="N174" s="16"/>
-      <c r="O174" s="16"/>
-      <c r="P174" s="16"/>
-      <c r="Q174" s="16"/>
-      <c r="R174" s="16"/>
-      <c r="S174" s="16"/>
-      <c r="T174" s="16"/>
-      <c r="U174" s="16"/>
-      <c r="V174" s="16"/>
-      <c r="W174" s="16"/>
-      <c r="X174" s="16"/>
-      <c r="Y174" s="16"/>
+      <c r="G174" s="15"/>
+      <c r="H174" s="15"/>
+      <c r="I174" s="15"/>
+      <c r="J174" s="15"/>
+      <c r="K174" s="15"/>
+      <c r="L174" s="15"/>
+      <c r="M174" s="15"/>
+      <c r="N174" s="15"/>
+      <c r="O174" s="15"/>
+      <c r="P174" s="15"/>
+      <c r="Q174" s="15"/>
+      <c r="R174" s="15"/>
+      <c r="S174" s="15"/>
+      <c r="T174" s="15"/>
+      <c r="U174" s="15"/>
+      <c r="V174" s="15"/>
+      <c r="W174" s="15"/>
+      <c r="X174" s="15"/>
+      <c r="Y174" s="15"/>
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="15" t="s">
+      <c r="A175" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B175" s="14" t="s">
+      <c r="B175" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="C175" s="14" t="s">
+      <c r="C175" s="13" t="s">
         <v>430</v>
       </c>
       <c r="D175" s="4"/>
@@ -8437,13 +8420,13 @@
       <c r="Y176" s="8"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="15" t="s">
+      <c r="A177" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B177" s="14" t="s">
+      <c r="B177" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="C177" s="14" t="s">
+      <c r="C177" s="13" t="s">
         <v>410</v>
       </c>
       <c r="D177" s="4"/>
@@ -8453,278 +8436,278 @@
       <c r="F177" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G177" s="16"/>
-      <c r="H177" s="16"/>
-      <c r="I177" s="16"/>
-      <c r="J177" s="16"/>
-      <c r="K177" s="16"/>
-      <c r="L177" s="16"/>
-      <c r="M177" s="16"/>
-      <c r="N177" s="16"/>
-      <c r="O177" s="16"/>
-      <c r="P177" s="16"/>
-      <c r="Q177" s="16"/>
-      <c r="R177" s="16"/>
-      <c r="S177" s="16"/>
-      <c r="T177" s="16"/>
-      <c r="U177" s="16"/>
-      <c r="V177" s="16"/>
-      <c r="W177" s="16"/>
-      <c r="X177" s="16"/>
-      <c r="Y177" s="16"/>
+      <c r="G177" s="15"/>
+      <c r="H177" s="15"/>
+      <c r="I177" s="15"/>
+      <c r="J177" s="15"/>
+      <c r="K177" s="15"/>
+      <c r="L177" s="15"/>
+      <c r="M177" s="15"/>
+      <c r="N177" s="15"/>
+      <c r="O177" s="15"/>
+      <c r="P177" s="15"/>
+      <c r="Q177" s="15"/>
+      <c r="R177" s="15"/>
+      <c r="S177" s="15"/>
+      <c r="T177" s="15"/>
+      <c r="U177" s="15"/>
+      <c r="V177" s="15"/>
+      <c r="W177" s="15"/>
+      <c r="X177" s="15"/>
+      <c r="Y177" s="15"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="15" t="s">
+      <c r="A178" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B178" s="14" t="s">
+      <c r="B178" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="C178" s="14" t="s">
+      <c r="C178" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="D178" s="16"/>
+      <c r="D178" s="15"/>
       <c r="E178" s="4" t="s">
         <v>437</v>
       </c>
       <c r="F178" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="G178" s="16"/>
-      <c r="H178" s="16"/>
-      <c r="I178" s="16"/>
-      <c r="J178" s="16"/>
-      <c r="K178" s="16"/>
-      <c r="L178" s="16"/>
-      <c r="M178" s="16"/>
-      <c r="N178" s="16"/>
-      <c r="O178" s="16"/>
-      <c r="P178" s="16"/>
-      <c r="Q178" s="16"/>
-      <c r="R178" s="16"/>
-      <c r="S178" s="16"/>
-      <c r="T178" s="16"/>
-      <c r="U178" s="16"/>
-      <c r="V178" s="16"/>
-      <c r="W178" s="16"/>
-      <c r="X178" s="16"/>
-      <c r="Y178" s="16"/>
+      <c r="G178" s="15"/>
+      <c r="H178" s="15"/>
+      <c r="I178" s="15"/>
+      <c r="J178" s="15"/>
+      <c r="K178" s="15"/>
+      <c r="L178" s="15"/>
+      <c r="M178" s="15"/>
+      <c r="N178" s="15"/>
+      <c r="O178" s="15"/>
+      <c r="P178" s="15"/>
+      <c r="Q178" s="15"/>
+      <c r="R178" s="15"/>
+      <c r="S178" s="15"/>
+      <c r="T178" s="15"/>
+      <c r="U178" s="15"/>
+      <c r="V178" s="15"/>
+      <c r="W178" s="15"/>
+      <c r="X178" s="15"/>
+      <c r="Y178" s="15"/>
     </row>
     <row r="179" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="17" t="s">
+      <c r="A179" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="B179" s="17" t="s">
+      <c r="B179" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="C179" s="18" t="s">
+      <c r="C179" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="D179" s="17"/>
-      <c r="E179" s="19" t="s">
+      <c r="D179" s="16"/>
+      <c r="E179" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="F179" s="17" t="s">
+      <c r="F179" s="16" t="s">
         <v>440</v>
       </c>
-      <c r="G179" s="17"/>
-      <c r="H179" s="17"/>
-      <c r="I179" s="17"/>
-      <c r="J179" s="17"/>
-      <c r="K179" s="17"/>
-      <c r="L179" s="17"/>
-      <c r="M179" s="17"/>
-      <c r="N179" s="17"/>
-      <c r="O179" s="17"/>
-      <c r="P179" s="17"/>
-      <c r="Q179" s="17"/>
-      <c r="R179" s="17"/>
-      <c r="S179" s="17"/>
-      <c r="T179" s="17"/>
-      <c r="U179" s="17"/>
-      <c r="V179" s="17"/>
-      <c r="W179" s="17"/>
-      <c r="X179" s="17"/>
-      <c r="Y179" s="17"/>
+      <c r="G179" s="16"/>
+      <c r="H179" s="16"/>
+      <c r="I179" s="16"/>
+      <c r="J179" s="16"/>
+      <c r="K179" s="16"/>
+      <c r="L179" s="16"/>
+      <c r="M179" s="16"/>
+      <c r="N179" s="16"/>
+      <c r="O179" s="16"/>
+      <c r="P179" s="16"/>
+      <c r="Q179" s="16"/>
+      <c r="R179" s="16"/>
+      <c r="S179" s="16"/>
+      <c r="T179" s="16"/>
+      <c r="U179" s="16"/>
+      <c r="V179" s="16"/>
+      <c r="W179" s="16"/>
+      <c r="X179" s="16"/>
+      <c r="Y179" s="16"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="20" t="s">
+      <c r="A180" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="B180" s="20" t="s">
+      <c r="B180" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="C180" s="20" t="s">
+      <c r="C180" s="19" t="s">
         <v>442</v>
       </c>
       <c r="D180" s="5"/>
-      <c r="E180" s="21" t="s">
+      <c r="E180" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="F180" s="20"/>
-      <c r="G180" s="20"/>
-      <c r="H180" s="20"/>
-      <c r="I180" s="20"/>
-      <c r="J180" s="20"/>
-      <c r="K180" s="20"/>
-      <c r="L180" s="20"/>
-      <c r="M180" s="20"/>
-      <c r="N180" s="20"/>
-      <c r="O180" s="20"/>
-      <c r="P180" s="20"/>
-      <c r="Q180" s="20"/>
-      <c r="R180" s="20"/>
-      <c r="S180" s="20"/>
-      <c r="T180" s="20"/>
-      <c r="U180" s="20"/>
-      <c r="V180" s="20"/>
-      <c r="W180" s="20"/>
-      <c r="X180" s="20"/>
-      <c r="Y180" s="20"/>
+      <c r="F180" s="19"/>
+      <c r="G180" s="19"/>
+      <c r="H180" s="19"/>
+      <c r="I180" s="19"/>
+      <c r="J180" s="19"/>
+      <c r="K180" s="19"/>
+      <c r="L180" s="19"/>
+      <c r="M180" s="19"/>
+      <c r="N180" s="19"/>
+      <c r="O180" s="19"/>
+      <c r="P180" s="19"/>
+      <c r="Q180" s="19"/>
+      <c r="R180" s="19"/>
+      <c r="S180" s="19"/>
+      <c r="T180" s="19"/>
+      <c r="U180" s="19"/>
+      <c r="V180" s="19"/>
+      <c r="W180" s="19"/>
+      <c r="X180" s="19"/>
+      <c r="Y180" s="19"/>
     </row>
     <row r="181" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="17" t="s">
+      <c r="A181" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="B181" s="17" t="s">
+      <c r="B181" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="C181" s="18" t="s">
+      <c r="C181" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="D181" s="17"/>
-      <c r="E181" s="19" t="s">
+      <c r="D181" s="16"/>
+      <c r="E181" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="F181" s="17" t="s">
+      <c r="F181" s="16" t="s">
         <v>440</v>
       </c>
-      <c r="G181" s="17"/>
-      <c r="H181" s="17"/>
-      <c r="I181" s="17"/>
-      <c r="J181" s="17"/>
-      <c r="K181" s="17"/>
-      <c r="L181" s="17"/>
-      <c r="M181" s="17"/>
-      <c r="N181" s="17"/>
-      <c r="O181" s="17"/>
-      <c r="P181" s="17"/>
-      <c r="Q181" s="17"/>
-      <c r="R181" s="17"/>
-      <c r="S181" s="17"/>
-      <c r="T181" s="17"/>
-      <c r="U181" s="17"/>
-      <c r="V181" s="17"/>
-      <c r="W181" s="17"/>
-      <c r="X181" s="17"/>
-      <c r="Y181" s="17"/>
+      <c r="G181" s="16"/>
+      <c r="H181" s="16"/>
+      <c r="I181" s="16"/>
+      <c r="J181" s="16"/>
+      <c r="K181" s="16"/>
+      <c r="L181" s="16"/>
+      <c r="M181" s="16"/>
+      <c r="N181" s="16"/>
+      <c r="O181" s="16"/>
+      <c r="P181" s="16"/>
+      <c r="Q181" s="16"/>
+      <c r="R181" s="16"/>
+      <c r="S181" s="16"/>
+      <c r="T181" s="16"/>
+      <c r="U181" s="16"/>
+      <c r="V181" s="16"/>
+      <c r="W181" s="16"/>
+      <c r="X181" s="16"/>
+      <c r="Y181" s="16"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="20" t="s">
+      <c r="A182" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="B182" s="20" t="s">
+      <c r="B182" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="C182" s="20" t="s">
+      <c r="C182" s="19" t="s">
         <v>446</v>
       </c>
       <c r="D182" s="5"/>
-      <c r="E182" s="21" t="s">
+      <c r="E182" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="F182" s="20"/>
-      <c r="G182" s="20"/>
-      <c r="H182" s="20"/>
-      <c r="I182" s="20"/>
-      <c r="J182" s="20"/>
-      <c r="K182" s="20"/>
-      <c r="L182" s="20"/>
-      <c r="M182" s="20"/>
-      <c r="N182" s="20"/>
-      <c r="O182" s="20"/>
-      <c r="P182" s="20"/>
-      <c r="Q182" s="20"/>
-      <c r="R182" s="20"/>
-      <c r="S182" s="20"/>
-      <c r="T182" s="20"/>
-      <c r="U182" s="20"/>
-      <c r="V182" s="20"/>
-      <c r="W182" s="20"/>
-      <c r="X182" s="20"/>
-      <c r="Y182" s="20"/>
-    </row>
-    <row r="183" s="25" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="22" t="s">
+      <c r="F182" s="19"/>
+      <c r="G182" s="19"/>
+      <c r="H182" s="19"/>
+      <c r="I182" s="19"/>
+      <c r="J182" s="19"/>
+      <c r="K182" s="19"/>
+      <c r="L182" s="19"/>
+      <c r="M182" s="19"/>
+      <c r="N182" s="19"/>
+      <c r="O182" s="19"/>
+      <c r="P182" s="19"/>
+      <c r="Q182" s="19"/>
+      <c r="R182" s="19"/>
+      <c r="S182" s="19"/>
+      <c r="T182" s="19"/>
+      <c r="U182" s="19"/>
+      <c r="V182" s="19"/>
+      <c r="W182" s="19"/>
+      <c r="X182" s="19"/>
+      <c r="Y182" s="19"/>
+    </row>
+    <row r="183" s="24" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A183" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B183" s="22" t="s">
+      <c r="B183" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="C183" s="23" t="s">
+      <c r="C183" s="22" t="s">
         <v>439</v>
       </c>
-      <c r="D183" s="22"/>
-      <c r="E183" s="24" t="s">
+      <c r="D183" s="21"/>
+      <c r="E183" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="F183" s="22" t="s">
+      <c r="F183" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="G183" s="22"/>
-      <c r="H183" s="22"/>
-      <c r="I183" s="22"/>
-      <c r="J183" s="22"/>
-      <c r="K183" s="22"/>
-      <c r="L183" s="22"/>
-      <c r="M183" s="22"/>
-      <c r="N183" s="22"/>
-      <c r="O183" s="22"/>
-      <c r="P183" s="22"/>
-      <c r="Q183" s="22"/>
-      <c r="R183" s="22"/>
-      <c r="S183" s="22"/>
-      <c r="T183" s="22"/>
-      <c r="U183" s="22"/>
-      <c r="V183" s="22"/>
-      <c r="W183" s="22"/>
-      <c r="X183" s="22"/>
-      <c r="Y183" s="22"/>
+      <c r="G183" s="21"/>
+      <c r="H183" s="21"/>
+      <c r="I183" s="21"/>
+      <c r="J183" s="21"/>
+      <c r="K183" s="21"/>
+      <c r="L183" s="21"/>
+      <c r="M183" s="21"/>
+      <c r="N183" s="21"/>
+      <c r="O183" s="21"/>
+      <c r="P183" s="21"/>
+      <c r="Q183" s="21"/>
+      <c r="R183" s="21"/>
+      <c r="S183" s="21"/>
+      <c r="T183" s="21"/>
+      <c r="U183" s="21"/>
+      <c r="V183" s="21"/>
+      <c r="W183" s="21"/>
+      <c r="X183" s="21"/>
+      <c r="Y183" s="21"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="20" t="s">
+      <c r="A184" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="B184" s="20" t="s">
+      <c r="B184" s="19" t="s">
         <v>448</v>
       </c>
-      <c r="C184" s="20" t="s">
+      <c r="C184" s="19" t="s">
         <v>449</v>
       </c>
       <c r="D184" s="5"/>
-      <c r="E184" s="21" t="s">
+      <c r="E184" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="F184" s="20"/>
-      <c r="G184" s="20"/>
-      <c r="H184" s="20"/>
-      <c r="I184" s="20"/>
-      <c r="J184" s="20"/>
-      <c r="K184" s="20"/>
-      <c r="L184" s="20"/>
-      <c r="M184" s="20"/>
-      <c r="N184" s="20"/>
-      <c r="O184" s="20"/>
-      <c r="P184" s="20"/>
-      <c r="Q184" s="20"/>
-      <c r="R184" s="20"/>
-      <c r="S184" s="20"/>
-      <c r="T184" s="20"/>
-      <c r="U184" s="20"/>
-      <c r="V184" s="20"/>
-      <c r="W184" s="20"/>
-      <c r="X184" s="20"/>
-      <c r="Y184" s="20"/>
+      <c r="F184" s="19"/>
+      <c r="G184" s="19"/>
+      <c r="H184" s="19"/>
+      <c r="I184" s="19"/>
+      <c r="J184" s="19"/>
+      <c r="K184" s="19"/>
+      <c r="L184" s="19"/>
+      <c r="M184" s="19"/>
+      <c r="N184" s="19"/>
+      <c r="O184" s="19"/>
+      <c r="P184" s="19"/>
+      <c r="Q184" s="19"/>
+      <c r="R184" s="19"/>
+      <c r="S184" s="19"/>
+      <c r="T184" s="19"/>
+      <c r="U184" s="19"/>
+      <c r="V184" s="19"/>
+      <c r="W184" s="19"/>
+      <c r="X184" s="19"/>
+      <c r="Y184" s="19"/>
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="4" t="s">
@@ -8756,31 +8739,31 @@
       <c r="Y185" s="8"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="26" t="s">
+      <c r="A186" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B186" s="26" t="s">
+      <c r="B186" s="25" t="s">
         <v>450</v>
       </c>
-      <c r="C186" s="26" t="s">
+      <c r="C186" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D186" s="27"/>
-      <c r="E186" s="27"/>
-      <c r="F186" s="26" t="s">
+      <c r="D186" s="26"/>
+      <c r="E186" s="26"/>
+      <c r="F186" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G186" s="27"/>
-      <c r="H186" s="27"/>
-      <c r="I186" s="27"/>
-      <c r="J186" s="27"/>
-      <c r="K186" s="27"/>
-      <c r="L186" s="27"/>
-      <c r="M186" s="27"/>
-      <c r="N186" s="27"/>
+      <c r="G186" s="26"/>
+      <c r="H186" s="26"/>
+      <c r="I186" s="26"/>
+      <c r="J186" s="26"/>
+      <c r="K186" s="26"/>
+      <c r="L186" s="26"/>
+      <c r="M186" s="26"/>
+      <c r="N186" s="26"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="28" t="s">
+      <c r="A187" s="27" t="s">
         <v>45</v>
       </c>
       <c r="B187" s="4" t="s">
@@ -8789,37 +8772,37 @@
       <c r="C187" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D187" s="29"/>
-      <c r="E187" s="30"/>
-      <c r="F187" s="30"/>
-      <c r="G187" s="30"/>
-      <c r="H187" s="30"/>
+      <c r="D187" s="28"/>
+      <c r="E187" s="29"/>
+      <c r="F187" s="29"/>
+      <c r="G187" s="29"/>
+      <c r="H187" s="29"/>
       <c r="I187" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="J187" s="30"/>
-      <c r="K187" s="30"/>
-      <c r="L187" s="30"/>
-      <c r="M187" s="30"/>
-      <c r="N187" s="30"/>
+      <c r="J187" s="29"/>
+      <c r="K187" s="29"/>
+      <c r="L187" s="29"/>
+      <c r="M187" s="29"/>
+      <c r="N187" s="29"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="31" t="s">
+      <c r="A188" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B188" s="27"/>
-      <c r="C188" s="27"/>
-      <c r="D188" s="27"/>
-      <c r="E188" s="27"/>
-      <c r="F188" s="27"/>
-      <c r="G188" s="27"/>
-      <c r="H188" s="27"/>
-      <c r="I188" s="27"/>
-      <c r="J188" s="27"/>
-      <c r="K188" s="27"/>
-      <c r="L188" s="27"/>
-      <c r="M188" s="27"/>
-      <c r="N188" s="27"/>
+      <c r="B188" s="26"/>
+      <c r="C188" s="26"/>
+      <c r="D188" s="26"/>
+      <c r="E188" s="26"/>
+      <c r="F188" s="26"/>
+      <c r="G188" s="26"/>
+      <c r="H188" s="26"/>
+      <c r="I188" s="26"/>
+      <c r="J188" s="26"/>
+      <c r="K188" s="26"/>
+      <c r="L188" s="26"/>
+      <c r="M188" s="26"/>
+      <c r="N188" s="26"/>
     </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -12488,1448 +12471,1449 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="84.7755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.311224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="131.122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.8367346938775"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.005102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="135.801020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>478</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>486</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>495</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>496</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>497</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>502</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>504</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>508</v>
       </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>510</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
         <v>513</v>
       </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
     </row>
     <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="13" t="s">
         <v>519</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>520</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="13" t="s">
         <v>519</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>521</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="13" t="s">
         <v>519</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>526</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C75" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="C76" s="14" t="s">
+      <c r="C76" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>528</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="14" t="s">
+      <c r="A83" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="14" t="s">
+      <c r="A85" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
     </row>
     <row r="86" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="14" t="s">
+      <c r="A86" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="14" t="s">
+      <c r="A87" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="14"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
+      <c r="A88" s="13"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="13" t="s">
         <v>486</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="14" t="s">
+      <c r="A91" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="14" t="s">
+      <c r="A92" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C92" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="14" t="s">
+      <c r="A93" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="14" t="s">
+      <c r="A94" s="13" t="s">
         <v>533</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C94" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
     </row>
     <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="14" t="s">
+      <c r="A96" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="C96" s="14" t="s">
+      <c r="C96" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="D96" s="14"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="14"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
     </row>
     <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="14" t="s">
+      <c r="A97" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C97" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
     </row>
     <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="14" t="s">
+      <c r="A98" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="C98" s="14" t="s">
+      <c r="C98" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
     </row>
     <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="14" t="s">
+      <c r="A99" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="13" t="s">
         <v>495</v>
       </c>
-      <c r="C99" s="14" t="s">
+      <c r="C99" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="D99" s="14"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="14"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="14" t="s">
+      <c r="A100" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>535</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" s="13" t="s">
         <v>536</v>
       </c>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
     </row>
     <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="14" t="s">
+      <c r="A101" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="C101" s="14" t="s">
+      <c r="C101" s="13" t="s">
         <v>538</v>
       </c>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
     </row>
     <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="14" t="s">
+      <c r="A102" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C102" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
     </row>
     <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="14" t="s">
+      <c r="A103" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="13" t="s">
         <v>497</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="14" t="s">
+      <c r="A104" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="C104" s="14" t="s">
+      <c r="C104" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
     </row>
     <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="14" t="s">
+      <c r="A105" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C105" s="14" t="s">
+      <c r="C105" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
     </row>
     <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="14" t="s">
+      <c r="A106" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="C106" s="14" t="s">
+      <c r="C106" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
     </row>
     <row r="107" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="14" t="s">
+      <c r="A107" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C107" s="13" t="s">
         <v>546</v>
       </c>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="14" t="s">
+      <c r="A108" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="C108" s="14" t="s">
+      <c r="C108" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="14" t="s">
+      <c r="A112" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C112" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C113" s="14" t="s">
+      <c r="C113" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
     </row>
     <row r="114" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="14" t="s">
+      <c r="A114" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B114" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="C114" s="14" t="s">
+      <c r="C114" s="13" t="s">
         <v>549</v>
       </c>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="14" t="s">
+      <c r="A115" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B115" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C115" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>550</v>
       </c>
-      <c r="B117" s="34" t="s">
+      <c r="B117" s="33" t="s">
         <v>551</v>
       </c>
       <c r="C117" s="0" t="s">
@@ -13940,7 +13924,7 @@
       <c r="A118" s="0" t="s">
         <v>550</v>
       </c>
-      <c r="B118" s="34" t="s">
+      <c r="B118" s="33" t="s">
         <v>553</v>
       </c>
       <c r="C118" s="0" t="s">
@@ -13951,7 +13935,7 @@
       <c r="A120" s="0" t="s">
         <v>555</v>
       </c>
-      <c r="B120" s="34" t="s">
+      <c r="B120" s="33" t="s">
         <v>556</v>
       </c>
       <c r="C120" s="0" t="s">
@@ -13962,7 +13946,7 @@
       <c r="A122" s="0" t="s">
         <v>558</v>
       </c>
-      <c r="B122" s="34" t="s">
+      <c r="B122" s="33" t="s">
         <v>559</v>
       </c>
       <c r="C122" s="0" t="s">
@@ -13973,7 +13957,7 @@
       <c r="A123" s="0" t="s">
         <v>558</v>
       </c>
-      <c r="B123" s="34" t="s">
+      <c r="B123" s="33" t="s">
         <v>561</v>
       </c>
       <c r="C123" s="0" t="s">
@@ -14003,60 +13987,60 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="14" t="s">
+      <c r="A129" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="13" t="s">
         <v>564</v>
       </c>
-      <c r="C129" s="14" t="s">
+      <c r="C129" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="14" t="s">
+      <c r="A130" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="13" t="s">
         <v>566</v>
       </c>
-      <c r="C130" s="14" t="s">
+      <c r="C130" s="13" t="s">
         <v>567</v>
       </c>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
     </row>
     <row r="132" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="35" t="s">
+      <c r="A132" s="34" t="s">
         <v>568</v>
       </c>
-      <c r="B132" s="14" t="s">
+      <c r="B132" s="13" t="s">
         <v>569</v>
       </c>
-      <c r="C132" s="14" t="s">
+      <c r="C132" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="D132" s="14"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
     </row>
     <row r="133" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="35" t="s">
+      <c r="A133" s="34" t="s">
         <v>568</v>
       </c>
-      <c r="B133" s="14" t="s">
+      <c r="B133" s="13" t="s">
         <v>570</v>
       </c>
-      <c r="C133" s="14" t="s">
+      <c r="C133" s="13" t="s">
         <v>571</v>
       </c>
-      <c r="D133" s="14"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14088,47 +14072,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>572</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>573</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>574</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>575</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>576</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>578</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>579</v>
       </c>
-      <c r="C2" s="36" t="n">
+      <c r="C2" s="35" t="n">
         <f aca="true">NOW()</f>
-        <v>44335.6544180116</v>
-      </c>
-      <c r="D2" s="14" t="s">
+        <v>44335.922903302</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>580</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>